<commit_message>
update & squashed important bug
</commit_message>
<xml_diff>
--- a/raw/cognition/raw_xlsx/Intervention timepoints - SPSS template.xlsx
+++ b/raw/cognition/raw_xlsx/Intervention timepoints - SPSS template.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">APC115-008</t>
   </si>
   <si>
-    <t xml:space="preserve">DECAF</t>
+    <t xml:space="preserve">CAF</t>
   </si>
   <si>
     <t xml:space="preserve">T2I</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">APC115-003</t>
   </si>
   <si>
-    <t xml:space="preserve">CAF</t>
+    <t xml:space="preserve">DECAF</t>
   </si>
   <si>
     <t xml:space="preserve">APC115-017</t>
@@ -294,15 +294,15 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2:Q125"/>
+      <selection pane="topLeft" activeCell="C73" activeCellId="0" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.86"/>

</xml_diff>